<commit_message>
In vitro validation 1
</commit_message>
<xml_diff>
--- a/Runs/Final_PDI1_RLU2/ARPE19/IV_Validation/Multiplex_Validation_set.xlsx
+++ b/Runs/Final_PDI1_RLU2/ARPE19/IV_Validation/Multiplex_Validation_set.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,97 +501,108 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Source_cell</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Double_bonds</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1816</v>
+        <v>12292</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>9.784000000000001</v>
+        <v>9.3028</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I2" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J2" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K2" t="n">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.02876492839171498</v>
+        <v>-0.03219976809333189</v>
       </c>
       <c r="M2" t="n">
-        <v>1.824533936810539</v>
-      </c>
-      <c r="N2" t="inlineStr"/>
+        <v>1.803581414630675</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>199</v>
+        <v>47698</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18PG</t>
+          <t>DSPC</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>9.3028</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3</v>
-      </c>
+        <v>6.12</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>6</v>
       </c>
       <c r="I3" t="n">
-        <v>350</v>
+        <v>20</v>
       </c>
       <c r="J3" t="n">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="K3" t="n">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.01178087292557521</v>
+        <v>-0.02821529602436637</v>
       </c>
       <c r="M3" t="n">
-        <v>1.928136675153991</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1</v>
-      </c>
+        <v>1.827886694251365</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4584</v>
+        <v>49643</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -604,59 +615,58 @@
       <c r="D4" t="n">
         <v>6.12</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
         <v>8</v>
       </c>
-      <c r="G4" t="n">
-        <v>36</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I4" t="n">
-        <v>40</v>
+        <v>450</v>
       </c>
       <c r="J4" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="K4" t="n">
-        <v>165</v>
+        <v>80</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.009366825235877736</v>
+        <v>-0.02254784829520736</v>
       </c>
       <c r="M4" t="n">
-        <v>1.942862366061146</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
+        <v>1.862458125399235</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1228</v>
+        <v>13512</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>9.784000000000001</v>
+        <v>9.3028</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I5" t="n">
         <v>40</v>
@@ -665,19 +675,24 @@
         <v>35</v>
       </c>
       <c r="K5" t="n">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.005714823075077572</v>
+        <v>-0.02076262833375528</v>
       </c>
       <c r="M5" t="n">
-        <v>1.965139579242027</v>
-      </c>
-      <c r="N5" t="inlineStr"/>
+        <v>1.873347967164093</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>888</v>
+        <v>2711</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -696,28 +711,33 @@
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I6" t="n">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="J6" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="K6" t="n">
-        <v>85</v>
+        <v>4</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.004108742822498138</v>
+        <v>-0.01909817385362694</v>
       </c>
       <c r="M6" t="n">
-        <v>1.974936668782761</v>
-      </c>
-      <c r="N6" t="inlineStr"/>
+        <v>1.883501139492876</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>744</v>
+        <v>305</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -736,152 +756,174 @@
       <c r="F7" t="n">
         <v>10</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>36</v>
+      </c>
       <c r="H7" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I7" t="n">
-        <v>40</v>
+        <v>350</v>
       </c>
       <c r="J7" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="K7" t="n">
-        <v>165</v>
+        <v>4</v>
       </c>
       <c r="L7" t="n">
-        <v>0.002542258098925915</v>
+        <v>-0.01178087292557521</v>
       </c>
       <c r="M7" t="n">
-        <v>2.015507774403448</v>
-      </c>
-      <c r="N7" t="n">
+        <v>1.928136675153991</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>95</v>
+        <v>22557</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18PG</t>
+          <t>DOPE</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>9.3028</v>
+        <v>9.784000000000001</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I8" t="n">
-        <v>350</v>
+        <v>50</v>
       </c>
       <c r="J8" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="K8" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="L8" t="n">
-        <v>0.002927333217570311</v>
+        <v>-0.01001357534436636</v>
       </c>
       <c r="M8" t="n">
-        <v>2.017856732627179</v>
-      </c>
-      <c r="N8" t="inlineStr"/>
+        <v>1.938917190399365</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3584</v>
+        <v>24965</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DSPC</t>
+          <t>DOPE</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>6.12</v>
+        <v>9.784000000000001</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I9" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J9" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="K9" t="n">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="L9" t="n">
-        <v>0.006805503251328551</v>
+        <v>-0.01001357534436636</v>
       </c>
       <c r="M9" t="n">
-        <v>2.041513569833104</v>
-      </c>
-      <c r="N9" t="inlineStr"/>
+        <v>1.938917190399365</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4080</v>
+        <v>27736</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DSPC</t>
+          <t>DOPE</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>6.12</v>
+        <v>9.784000000000001</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I10" t="n">
         <v>40</v>
       </c>
       <c r="J10" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K10" t="n">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="L10" t="n">
-        <v>0.00701378717148632</v>
+        <v>-0.005617059102730622</v>
       </c>
       <c r="M10" t="n">
-        <v>2.042784101746066</v>
-      </c>
-      <c r="N10" t="inlineStr"/>
+        <v>1.965735939473343</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>970</v>
+        <v>5265</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -894,34 +936,43 @@
       <c r="D11" t="n">
         <v>9.3028</v>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
       <c r="F11" t="n">
         <v>10</v>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>36</v>
+      </c>
       <c r="H11" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I11" t="n">
-        <v>250</v>
+        <v>30</v>
       </c>
       <c r="J11" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="K11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L11" t="n">
-        <v>0.007812100924060301</v>
+        <v>-0.005086681177133375</v>
       </c>
       <c r="M11" t="n">
-        <v>2.047653815636768</v>
-      </c>
-      <c r="N11" t="inlineStr"/>
+        <v>1.968971244819486</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>969</v>
+        <v>7506</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -940,198 +991,221 @@
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I12" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="J12" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="K12" t="n">
         <v>4</v>
       </c>
       <c r="L12" t="n">
-        <v>0.007812100924060301</v>
+        <v>-0.005086681177133375</v>
       </c>
       <c r="M12" t="n">
-        <v>2.047653815636768</v>
-      </c>
-      <c r="N12" t="inlineStr"/>
+        <v>1.968971244819486</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>404</v>
+        <v>52416</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>18PG</t>
+          <t>DSPC</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>9.3028</v>
+        <v>6.12</v>
       </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>10</v>
-      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I13" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J13" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="K13" t="n">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="L13" t="n">
-        <v>0.01181481204045297</v>
+        <v>-0.002812502040508305</v>
       </c>
       <c r="M13" t="n">
-        <v>2.072070353446763</v>
-      </c>
-      <c r="N13" t="inlineStr"/>
+        <v>1.982843737552899</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1372</v>
+        <v>12059</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>9.784000000000001</v>
-      </c>
-      <c r="E14" t="inlineStr"/>
+        <v>9.3028</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
       <c r="F14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I14" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J14" t="n">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="K14" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L14" t="n">
-        <v>0.01435366246021119</v>
+        <v>0.003519527818827326</v>
       </c>
       <c r="M14" t="n">
-        <v>2.087557341007288</v>
-      </c>
-      <c r="N14" t="inlineStr"/>
+        <v>2.021469119694847</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1823</v>
+        <v>53928</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DSPC</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>9.784000000000001</v>
-      </c>
-      <c r="E15" t="n">
-        <v>2</v>
-      </c>
+        <v>6.12</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>9</v>
-      </c>
-      <c r="G15" t="n">
-        <v>36</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I15" t="n">
-        <v>350</v>
+        <v>20</v>
       </c>
       <c r="J15" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="K15" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L15" t="n">
-        <v>0.01519848831312965</v>
+        <v>0.005509368166202438</v>
       </c>
       <c r="M15" t="n">
-        <v>2.092710778710091</v>
-      </c>
-      <c r="N15" t="n">
-        <v>2</v>
-      </c>
+        <v>2.033607145813835</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2436</v>
+        <v>45502</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>DSPC</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>12.515</v>
+        <v>6.12</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G16" t="n">
         <v>36</v>
       </c>
       <c r="H16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I16" t="n">
         <v>40</v>
       </c>
       <c r="J16" t="n">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="K16" t="n">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="L16" t="n">
-        <v>0.03377624604754183</v>
+        <v>0.009176832779749148</v>
       </c>
       <c r="M16" t="n">
-        <v>2.206035100890005</v>
-      </c>
-      <c r="N16" t="inlineStr"/>
+        <v>2.055978679956469</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1045</v>
+        <v>5419</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1144,38 +1218,39 @@
       <c r="D17" t="n">
         <v>9.3028</v>
       </c>
-      <c r="E17" t="n">
-        <v>3</v>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
         <v>10</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I17" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="J17" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="K17" t="n">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="L17" t="n">
-        <v>0.04238591311351571</v>
+        <v>0.01133304251081966</v>
       </c>
       <c r="M17" t="n">
-        <v>2.258554069992446</v>
-      </c>
-      <c r="N17" t="n">
-        <v>1</v>
-      </c>
+        <v>2.069131559316</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>624</v>
+        <v>10332</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1188,636 +1263,721 @@
       <c r="D18" t="n">
         <v>9.3028</v>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I18" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J18" t="n">
         <v>25</v>
       </c>
       <c r="K18" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0513829146071688</v>
+        <v>0.01133304251081966</v>
       </c>
       <c r="M18" t="n">
-        <v>2.31343577910373</v>
-      </c>
-      <c r="N18" t="n">
+        <v>2.069131559316</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>4228</v>
+        <v>2240</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DSPC</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>6.12</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>8</v>
-      </c>
+        <v>9.3028</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I19" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J19" t="n">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="K19" t="n">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="L19" t="n">
-        <v>0.05657447402818059</v>
+        <v>0.01229540504241102</v>
       </c>
       <c r="M19" t="n">
-        <v>2.345104291571902</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0</v>
+        <v>2.075001970758707</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2392</v>
+        <v>481</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>12.515</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
+        <v>9.3028</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
         <v>5</v>
       </c>
       <c r="I20" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J20" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="K20" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="L20" t="n">
-        <v>0.08846259517946339</v>
+        <v>0.01230942277791353</v>
       </c>
       <c r="M20" t="n">
-        <v>2.539621830594727</v>
-      </c>
-      <c r="N20" t="n">
-        <v>2</v>
-      </c>
+        <v>2.075087478945273</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>5375</v>
+        <v>4793</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14PA</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>11.8502</v>
+        <v>9.3028</v>
       </c>
       <c r="E21" t="n">
+        <v>3</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="n">
+        <v>7</v>
+      </c>
+      <c r="I21" t="n">
+        <v>70</v>
+      </c>
+      <c r="J21" t="n">
+        <v>25</v>
+      </c>
+      <c r="K21" t="n">
         <v>2</v>
       </c>
-      <c r="F21" t="n">
-        <v>8</v>
-      </c>
-      <c r="G21" t="n">
-        <v>28</v>
-      </c>
-      <c r="H21" t="n">
-        <v>9</v>
-      </c>
-      <c r="I21" t="n">
-        <v>350</v>
-      </c>
-      <c r="J21" t="n">
-        <v>75</v>
-      </c>
-      <c r="K21" t="n">
-        <v>165</v>
-      </c>
       <c r="L21" t="n">
-        <v>0.09946681989704756</v>
+        <v>0.01982090196172159</v>
       </c>
       <c r="M21" t="n">
-        <v>2.60674760137199</v>
-      </c>
-      <c r="N21" t="n">
-        <v>0</v>
+        <v>2.120907501966502</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>4704</v>
+        <v>21292</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>14PA</t>
+          <t>DOPE</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>11.8502</v>
+        <v>9.784000000000001</v>
       </c>
       <c r="E22" t="n">
         <v>2</v>
       </c>
       <c r="F22" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G22" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H22" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I22" t="n">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="J22" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="K22" t="n">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="L22" t="n">
-        <v>0.1087179072094666</v>
+        <v>0.02216031457127846</v>
       </c>
       <c r="M22" t="n">
-        <v>2.663179233977746</v>
-      </c>
-      <c r="N22" t="inlineStr"/>
+        <v>2.135177918884799</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>4751</v>
+        <v>11961</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>14PA</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>11.8502</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+        <v>9.3028</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10</v>
+      </c>
+      <c r="G23" t="n">
+        <v>36</v>
+      </c>
       <c r="H23" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I23" t="n">
-        <v>350</v>
+        <v>70</v>
       </c>
       <c r="J23" t="n">
         <v>75</v>
       </c>
       <c r="K23" t="n">
-        <v>85</v>
+        <v>180</v>
       </c>
       <c r="L23" t="n">
-        <v>0.1235658295712452</v>
+        <v>0.02689751678710435</v>
       </c>
       <c r="M23" t="n">
-        <v>2.753751560384595</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0</v>
+        <v>2.164074852401336</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>5208</v>
+        <v>77997</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>14PA</t>
+          <t>DDAB</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>11.8502</v>
+        <v>12.73</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I24" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J24" t="n">
         <v>25</v>
       </c>
       <c r="K24" t="n">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1573440141678602</v>
+        <v>0.03202223787543083</v>
       </c>
       <c r="M24" t="n">
-        <v>2.959798486423947</v>
-      </c>
-      <c r="N24" t="n">
+        <v>2.195335651040128</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>5928</v>
+        <v>11975</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>DDAB</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>12.73</v>
-      </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+        <v>9.3028</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3</v>
+      </c>
+      <c r="F25" t="n">
+        <v>10</v>
+      </c>
+      <c r="G25" t="n">
+        <v>36</v>
+      </c>
       <c r="H25" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I25" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J25" t="n">
         <v>25</v>
       </c>
       <c r="K25" t="n">
-        <v>165</v>
+        <v>2</v>
       </c>
       <c r="L25" t="n">
-        <v>0.1671856253705378</v>
+        <v>0.03458718978383925</v>
       </c>
       <c r="M25" t="n">
-        <v>3.019832314760281</v>
-      </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
+        <v>2.21098185768142</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>5734</v>
+        <v>37802</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>14PA</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>11.8502</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
+        <v>12.515</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4</v>
+      </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I26" t="n">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="J26" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="K26" t="n">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="L26" t="n">
-        <v>0.1711164088406764</v>
+        <v>0.04670055652087007</v>
       </c>
       <c r="M26" t="n">
-        <v>3.043810093928126</v>
-      </c>
-      <c r="N26" t="n">
-        <v>0</v>
+        <v>2.284873394777307</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O26" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2516</v>
+        <v>7653</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>12.515</v>
+        <v>9.3028</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I27" t="n">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="J27" t="n">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="K27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L27" t="n">
-        <v>0.1977052878815564</v>
+        <v>0.08839668455763268</v>
       </c>
       <c r="M27" t="n">
-        <v>3.206002256077494</v>
-      </c>
-      <c r="N27" t="n">
-        <v>2</v>
+        <v>2.539219775801559</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1610</v>
+        <v>10824</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>9.784000000000001</v>
-      </c>
-      <c r="E28" t="n">
-        <v>2</v>
-      </c>
-      <c r="F28" t="n">
-        <v>9</v>
-      </c>
-      <c r="G28" t="n">
-        <v>36</v>
-      </c>
+        <v>9.3028</v>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I28" t="n">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="J28" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="K28" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="L28" t="n">
-        <v>0.2826836714986803</v>
+        <v>0.1175675363482386</v>
       </c>
       <c r="M28" t="n">
-        <v>3.72437039614195</v>
-      </c>
-      <c r="N28" t="inlineStr"/>
+        <v>2.717161971724255</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>258</v>
+        <v>43165</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>18PG</t>
+          <t>DSPC</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>9.3028</v>
-      </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+        <v>6.12</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>8</v>
+      </c>
+      <c r="G29" t="n">
+        <v>36</v>
+      </c>
       <c r="H29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I29" t="n">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="J29" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K29" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="L29" t="n">
-        <v>0.3253524932584978</v>
+        <v>0.1617752934029897</v>
       </c>
       <c r="M29" t="n">
-        <v>3.984650208876837</v>
-      </c>
-      <c r="N29" t="n">
-        <v>1</v>
+        <v>2.986829289758237</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>5431</v>
+        <v>5166</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>14PA</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>11.8502</v>
+        <v>9.3028</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G30" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H30" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I30" t="n">
-        <v>350</v>
+        <v>20</v>
       </c>
       <c r="J30" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K30" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="L30" t="n">
-        <v>0.3358896452931631</v>
+        <v>0.1925725490109248</v>
       </c>
       <c r="M30" t="n">
-        <v>4.048926836288294</v>
-      </c>
-      <c r="N30" t="inlineStr"/>
+        <v>3.174692548966641</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2103</v>
+        <v>62904</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>14PA</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>9.784000000000001</v>
+        <v>11.8502</v>
       </c>
       <c r="E31" t="n">
         <v>2</v>
       </c>
       <c r="F31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H31" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I31" t="n">
-        <v>350</v>
+        <v>40</v>
       </c>
       <c r="J31" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="K31" t="n">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="L31" t="n">
-        <v>0.3522075903937099</v>
+        <v>0.2414184786010612</v>
       </c>
       <c r="M31" t="n">
-        <v>4.148466301401631</v>
-      </c>
-      <c r="N31" t="n">
-        <v>2</v>
-      </c>
+        <v>3.472652719466473</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>5150</v>
+        <v>9159</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14PA</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>11.8502</v>
+        <v>9.3028</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G32" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H32" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I32" t="n">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="J32" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="K32" t="n">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="L32" t="n">
-        <v>0.4192485273127374</v>
+        <v>0.2600994423937644</v>
       </c>
       <c r="M32" t="n">
-        <v>4.557416016607698</v>
-      </c>
-      <c r="N32" t="n">
-        <v>0</v>
+        <v>3.586606598601963</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2894</v>
+        <v>29038</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1830,40 +1990,39 @@
       <c r="D33" t="n">
         <v>12.515</v>
       </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>4</v>
-      </c>
-      <c r="G33" t="n">
-        <v>36</v>
-      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I33" t="n">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="J33" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K33" t="n">
         <v>4</v>
       </c>
       <c r="L33" t="n">
-        <v>0.5089090321312522</v>
+        <v>0.2936191166443746</v>
       </c>
       <c r="M33" t="n">
-        <v>5.104345096000638</v>
-      </c>
-      <c r="N33" t="n">
+        <v>3.791076611530685</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O33" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>5099</v>
+        <v>62723</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1889,69 +2048,81 @@
         <v>7</v>
       </c>
       <c r="I34" t="n">
-        <v>350</v>
+        <v>50</v>
       </c>
       <c r="J34" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="K34" t="n">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="L34" t="n">
-        <v>0.5298632406640909</v>
+        <v>0.3164294396673574</v>
       </c>
       <c r="M34" t="n">
-        <v>5.232165768050954</v>
-      </c>
-      <c r="N34" t="inlineStr"/>
+        <v>3.93021958197088</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>3282</v>
+        <v>21125</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>DOPE</t>
         </is>
       </c>
       <c r="C35" t="n">
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>12.515</v>
+        <v>9.784000000000001</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G35" t="n">
         <v>36</v>
       </c>
       <c r="H35" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I35" t="n">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="J35" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K35" t="n">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="L35" t="n">
-        <v>0.5621432586403099</v>
+        <v>0.3291553833186111</v>
       </c>
       <c r="M35" t="n">
-        <v>5.42907387770589</v>
-      </c>
-      <c r="N35" t="inlineStr"/>
+        <v>4.007847838243527</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O35" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>3329</v>
+        <v>33632</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1964,51 +2135,62 @@
       <c r="D36" t="n">
         <v>12.515</v>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4</v>
+      </c>
+      <c r="G36" t="n">
+        <v>36</v>
+      </c>
       <c r="H36" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I36" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J36" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="K36" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="L36" t="n">
-        <v>0.5665209134426206</v>
+        <v>0.3398394047111878</v>
       </c>
       <c r="M36" t="n">
-        <v>5.455777571999985</v>
-      </c>
-      <c r="N36" t="n">
+        <v>4.073020368738245</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O36" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1550</v>
+        <v>34014</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C37" t="n">
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>9.784000000000001</v>
+        <v>12.515</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G37" t="n">
         <v>36</v>
@@ -2017,65 +2199,81 @@
         <v>7</v>
       </c>
       <c r="I37" t="n">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="J37" t="n">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="K37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L37" t="n">
-        <v>0.5843347686434741</v>
+        <v>0.3398394047111878</v>
       </c>
       <c r="M37" t="n">
-        <v>5.564442088725191</v>
-      </c>
-      <c r="N37" t="inlineStr"/>
+        <v>4.073020368738245</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1937</v>
+        <v>38313</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>9.784000000000001</v>
-      </c>
-      <c r="E38" t="inlineStr"/>
+        <v>12.515</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
       <c r="F38" t="n">
-        <v>9</v>
-      </c>
-      <c r="G38" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="G38" t="n">
+        <v>36</v>
+      </c>
       <c r="H38" t="n">
         <v>10</v>
       </c>
       <c r="I38" t="n">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="J38" t="n">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="K38" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L38" t="n">
-        <v>0.5843347686434741</v>
+        <v>0.3582579278154162</v>
       </c>
       <c r="M38" t="n">
-        <v>5.564442088725191</v>
-      </c>
-      <c r="N38" t="inlineStr"/>
+        <v>4.185373359674038</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O38" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3283</v>
+        <v>33663</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -2098,158 +2296,178 @@
         <v>36</v>
       </c>
       <c r="H39" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I39" t="n">
-        <v>350</v>
+        <v>90</v>
       </c>
       <c r="J39" t="n">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="K39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L39" t="n">
-        <v>0.6032974601224074</v>
+        <v>0.3582579278154162</v>
       </c>
       <c r="M39" t="n">
-        <v>5.680114506746684</v>
-      </c>
-      <c r="N39" t="n">
+        <v>4.185373359674038</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O39" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>5989</v>
+        <v>35914</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>DDAB</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C40" t="n">
         <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>12.73</v>
+        <v>12.515</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="G40" t="n">
+        <v>36</v>
+      </c>
       <c r="H40" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I40" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J40" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="K40" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L40" t="n">
-        <v>0.6081081301613704</v>
+        <v>0.3582579278154162</v>
       </c>
       <c r="M40" t="n">
-        <v>5.709459593984359</v>
-      </c>
-      <c r="N40" t="n">
-        <v>0</v>
-      </c>
+        <v>4.185373359674038</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2503</v>
+        <v>747</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>12.515</v>
+        <v>9.3028</v>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I41" t="n">
-        <v>350</v>
+        <v>70</v>
       </c>
       <c r="J41" t="n">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="K41" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L41" t="n">
-        <v>0.6703159841735342</v>
+        <v>0.3607029439323729</v>
       </c>
       <c r="M41" t="n">
-        <v>6.088927503458558</v>
-      </c>
-      <c r="N41" t="n">
-        <v>2</v>
+        <v>4.200287957987475</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O41" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>3078</v>
+        <v>59979</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>14PA</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>12.515</v>
+        <v>11.8502</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
-        <v>4</v>
-      </c>
-      <c r="G42" t="n">
-        <v>36</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I42" t="n">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="J42" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L42" t="n">
-        <v>0.6783975798586739</v>
+        <v>0.409514679956245</v>
       </c>
       <c r="M42" t="n">
-        <v>6.13822523713791</v>
-      </c>
-      <c r="N42" t="inlineStr"/>
+        <v>4.498039547733094</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2697</v>
+        <v>33974</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -2275,151 +2493,167 @@
         <v>7</v>
       </c>
       <c r="I43" t="n">
-        <v>70</v>
+        <v>250</v>
       </c>
       <c r="J43" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="K43" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L43" t="n">
-        <v>0.6783975798586739</v>
+        <v>0.5089090321312522</v>
       </c>
       <c r="M43" t="n">
-        <v>6.13822523713791</v>
-      </c>
-      <c r="N43" t="n">
+        <v>5.104345096000638</v>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O43" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1358</v>
+        <v>33757</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C44" t="n">
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>9.784000000000001</v>
+        <v>12.515</v>
       </c>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" t="n">
-        <v>9</v>
-      </c>
+      <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I44" t="n">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="J44" t="n">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="K44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L44" t="n">
-        <v>0.6803965636544311</v>
+        <v>0.5239489535343306</v>
       </c>
       <c r="M44" t="n">
-        <v>6.150419038292029</v>
-      </c>
-      <c r="N44" t="inlineStr"/>
+        <v>5.196088616559416</v>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O44" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>3083</v>
+        <v>77583</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>DDAB</t>
         </is>
       </c>
       <c r="C45" t="n">
         <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>12.515</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>4</v>
-      </c>
-      <c r="G45" t="n">
-        <v>36</v>
-      </c>
+        <v>12.73</v>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I45" t="n">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="J45" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="K45" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L45" t="n">
-        <v>0.6854022595915614</v>
+        <v>0.5476054727148189</v>
       </c>
       <c r="M45" t="n">
-        <v>6.180953783508524</v>
-      </c>
-      <c r="N45" t="inlineStr"/>
+        <v>5.340393383560395</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1739</v>
+        <v>3690</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>18PG</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>9.784000000000001</v>
+        <v>9.3028</v>
       </c>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="n">
-        <v>9</v>
-      </c>
+      <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I46" t="n">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="J46" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="K46" t="n">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="L46" t="n">
-        <v>0.6894352547425637</v>
+        <v>0.570486804247844</v>
       </c>
       <c r="M46" t="n">
-        <v>6.205555053929639</v>
-      </c>
-      <c r="N46" t="inlineStr"/>
+        <v>5.479969505911848</v>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2317</v>
+        <v>31499</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -2436,50 +2670,59 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I47" t="n">
-        <v>70</v>
+        <v>450</v>
       </c>
       <c r="J47" t="n">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="K47" t="n">
         <v>4</v>
       </c>
       <c r="L47" t="n">
-        <v>0.6914390322028703</v>
+        <v>0.5714983044792054</v>
       </c>
       <c r="M47" t="n">
-        <v>6.217778096437509</v>
-      </c>
-      <c r="N47" t="n">
+        <v>5.486139657323152</v>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O47" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5969</v>
+        <v>21886</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>DDAB</t>
+          <t>DOPE</t>
         </is>
       </c>
       <c r="C48" t="n">
         <v>1</v>
       </c>
       <c r="D48" t="n">
-        <v>12.73</v>
-      </c>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" t="n">
+        <v>9</v>
+      </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I48" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J48" t="n">
         <v>65</v>
@@ -2488,18 +2731,23 @@
         <v>4</v>
       </c>
       <c r="L48" t="n">
-        <v>0.6914390322028703</v>
+        <v>0.5843347686434741</v>
       </c>
       <c r="M48" t="n">
-        <v>6.217778096437509</v>
-      </c>
-      <c r="N48" t="n">
-        <v>0</v>
+        <v>5.564442088725191</v>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O48" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1749</v>
+        <v>19620</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -2520,374 +2768,423 @@
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I49" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="J49" t="n">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="K49" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L49" t="n">
-        <v>0.6995979820208831</v>
+        <v>0.5843347686434741</v>
       </c>
       <c r="M49" t="n">
-        <v>6.267547690327386</v>
-      </c>
-      <c r="N49" t="n">
+        <v>5.564442088725191</v>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O49" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>3126</v>
+        <v>72778</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>DDAB</t>
         </is>
       </c>
       <c r="C50" t="n">
         <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>12.515</v>
+        <v>12.73</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>4</v>
-      </c>
-      <c r="G50" t="n">
-        <v>36</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I50" t="n">
-        <v>250</v>
+        <v>80</v>
       </c>
       <c r="J50" t="n">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="K50" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="L50" t="n">
-        <v>0.7153169160468854</v>
+        <v>0.6081081301613704</v>
       </c>
       <c r="M50" t="n">
-        <v>6.363433187886001</v>
-      </c>
-      <c r="N50" t="n">
-        <v>2</v>
+        <v>5.709459593984359</v>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2721</v>
+        <v>74936</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>DDAB</t>
         </is>
       </c>
       <c r="C51" t="n">
         <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>12.515</v>
+        <v>12.73</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>4</v>
-      </c>
-      <c r="G51" t="n">
-        <v>36</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I51" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="J51" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="K51" t="n">
         <v>7</v>
       </c>
       <c r="L51" t="n">
-        <v>0.7153169160468854</v>
+        <v>0.6081081301613704</v>
       </c>
       <c r="M51" t="n">
-        <v>6.363433187886001</v>
-      </c>
-      <c r="N51" t="n">
-        <v>2</v>
+        <v>5.709459593984359</v>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1159</v>
+        <v>36322</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C52" t="n">
         <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>9.784000000000001</v>
-      </c>
-      <c r="E52" t="inlineStr"/>
+        <v>12.515</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
       <c r="F52" t="n">
+        <v>4</v>
+      </c>
+      <c r="G52" t="n">
+        <v>36</v>
+      </c>
+      <c r="H52" t="n">
         <v>9</v>
       </c>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="n">
-        <v>5</v>
-      </c>
       <c r="I52" t="n">
-        <v>350</v>
+        <v>80</v>
       </c>
       <c r="J52" t="n">
         <v>35</v>
       </c>
       <c r="K52" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L52" t="n">
-        <v>0.7202404058665945</v>
+        <v>0.6783975798586739</v>
       </c>
       <c r="M52" t="n">
-        <v>6.393466475786226</v>
-      </c>
-      <c r="N52" t="inlineStr"/>
+        <v>6.13822523713791</v>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1163</v>
+        <v>33674</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C53" t="n">
         <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>9.784000000000001</v>
-      </c>
-      <c r="E53" t="inlineStr"/>
+        <v>12.515</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
       <c r="F53" t="n">
-        <v>9</v>
-      </c>
-      <c r="G53" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="G53" t="n">
+        <v>36</v>
+      </c>
       <c r="H53" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I53" t="n">
-        <v>350</v>
+        <v>60</v>
       </c>
       <c r="J53" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="K53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L53" t="n">
-        <v>0.7202404058665945</v>
+        <v>0.6783975798586739</v>
       </c>
       <c r="M53" t="n">
-        <v>6.393466475786226</v>
-      </c>
-      <c r="N53" t="inlineStr"/>
+        <v>6.13822523713791</v>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1381</v>
+        <v>36100</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C54" t="n">
         <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>9.784000000000001</v>
+        <v>12.515</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
+        <v>4</v>
+      </c>
+      <c r="G54" t="n">
+        <v>36</v>
+      </c>
+      <c r="H54" t="n">
         <v>9</v>
       </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="n">
-        <v>6</v>
-      </c>
       <c r="I54" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="J54" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K54" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L54" t="n">
-        <v>0.7385985299268407</v>
+        <v>0.6783975798586739</v>
       </c>
       <c r="M54" t="n">
-        <v>6.505451032553728</v>
-      </c>
-      <c r="N54" t="n">
-        <v>2</v>
-      </c>
+        <v>6.13822523713791</v>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1193</v>
+        <v>36099</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C55" t="n">
         <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>9.784000000000001</v>
+        <v>12.515</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
+        <v>4</v>
+      </c>
+      <c r="G55" t="n">
+        <v>36</v>
+      </c>
+      <c r="H55" t="n">
         <v>9</v>
       </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="n">
-        <v>5</v>
-      </c>
       <c r="I55" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J55" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="K55" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L55" t="n">
-        <v>0.7385985299268407</v>
+        <v>0.6783975798586739</v>
       </c>
       <c r="M55" t="n">
-        <v>6.505451032553728</v>
-      </c>
-      <c r="N55" t="n">
-        <v>2</v>
-      </c>
+        <v>6.13822523713791</v>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>HepG2</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2305</v>
+        <v>14584</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>DOPE</t>
         </is>
       </c>
       <c r="C56" t="n">
         <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>12.515</v>
+        <v>9.784000000000001</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
-        <v>4</v>
-      </c>
-      <c r="G56" t="n">
-        <v>36</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
         <v>5</v>
       </c>
       <c r="I56" t="n">
-        <v>70</v>
+        <v>250</v>
       </c>
       <c r="J56" t="n">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="K56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L56" t="n">
-        <v>0.8422277437855306</v>
+        <v>0.6803965636544311</v>
       </c>
       <c r="M56" t="n">
-        <v>7.137589237091737</v>
-      </c>
-      <c r="N56" t="inlineStr"/>
+        <v>6.150419038292029</v>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O56" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2581</v>
+        <v>17115</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DOTAP</t>
+          <t>DOPE</t>
         </is>
       </c>
       <c r="C57" t="n">
         <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>12.515</v>
+        <v>9.784000000000001</v>
       </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
         <v>6</v>
       </c>
       <c r="I57" t="n">
+        <v>90</v>
+      </c>
+      <c r="J57" t="n">
         <v>70</v>
       </c>
-      <c r="J57" t="n">
-        <v>55</v>
-      </c>
       <c r="K57" t="n">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="L57" t="n">
-        <v>0.8703719264843812</v>
+        <v>0.6803965636544311</v>
       </c>
       <c r="M57" t="n">
-        <v>7.309268751554725</v>
-      </c>
-      <c r="N57" t="inlineStr"/>
+        <v>6.150419038292029</v>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2106</v>
+        <v>14566</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -2906,28 +3203,33 @@
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I58" t="n">
-        <v>250</v>
+        <v>80</v>
       </c>
       <c r="J58" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K58" t="n">
-        <v>165</v>
+        <v>3</v>
       </c>
       <c r="L58" t="n">
-        <v>0.8790140722709167</v>
+        <v>0.6803965636544311</v>
       </c>
       <c r="M58" t="n">
-        <v>7.361985840852591</v>
-      </c>
-      <c r="N58" t="inlineStr"/>
+        <v>6.150419038292029</v>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1513</v>
+        <v>17213</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2949,101 +3251,672 @@
         <v>6</v>
       </c>
       <c r="I59" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J59" t="n">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="K59" t="n">
-        <v>165</v>
+        <v>5</v>
       </c>
       <c r="L59" t="n">
-        <v>0.8806656720833289</v>
+        <v>0.6803965636544311</v>
       </c>
       <c r="M59" t="n">
-        <v>7.372060599708306</v>
-      </c>
-      <c r="N59" t="inlineStr"/>
+        <v>6.150419038292029</v>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>3505</v>
+        <v>28991</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>DSPC</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C60" t="n">
         <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>6.12</v>
-      </c>
-      <c r="E60" t="inlineStr"/>
+        <v>12.515</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
       <c r="F60" t="n">
-        <v>8</v>
-      </c>
-      <c r="G60" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="G60" t="n">
+        <v>36</v>
+      </c>
       <c r="H60" t="n">
         <v>5</v>
       </c>
       <c r="I60" t="n">
-        <v>70</v>
+        <v>350</v>
       </c>
       <c r="J60" t="n">
         <v>25</v>
       </c>
       <c r="K60" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="L60" t="n">
-        <v>0.901182782246763</v>
+        <v>0.6868711968685431</v>
       </c>
       <c r="M60" t="n">
-        <v>7.497214971705254</v>
-      </c>
-      <c r="N60" t="inlineStr"/>
+        <v>6.189914300898113</v>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O60" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1333</v>
+        <v>29214</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>DOPE</t>
+          <t>DOTAP</t>
         </is>
       </c>
       <c r="C61" t="n">
         <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>9.784000000000001</v>
+        <v>12.515</v>
       </c>
       <c r="E61" t="inlineStr"/>
-      <c r="F61" t="n">
-        <v>9</v>
-      </c>
+      <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
         <v>5</v>
       </c>
       <c r="I61" t="n">
+        <v>250</v>
+      </c>
+      <c r="J61" t="n">
         <v>70</v>
       </c>
-      <c r="J61" t="n">
+      <c r="K61" t="n">
+        <v>5</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0.6914390322028703</v>
+      </c>
+      <c r="M61" t="n">
+        <v>6.217778096437509</v>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O61" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>19525</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="n">
+        <v>9</v>
+      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="n">
+        <v>7</v>
+      </c>
+      <c r="I62" t="n">
+        <v>200</v>
+      </c>
+      <c r="J62" t="n">
+        <v>75</v>
+      </c>
+      <c r="K62" t="n">
+        <v>4</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0.6995979820208831</v>
+      </c>
+      <c r="M62" t="n">
+        <v>6.267547690327386</v>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>19359</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>9</v>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="n">
+        <v>7</v>
+      </c>
+      <c r="I63" t="n">
+        <v>350</v>
+      </c>
+      <c r="J63" t="n">
         <v>55</v>
       </c>
-      <c r="K61" t="n">
-        <v>165</v>
-      </c>
-      <c r="L61" t="n">
-        <v>0.950788716592841</v>
-      </c>
-      <c r="M61" t="n">
-        <v>7.79981117121633</v>
-      </c>
-      <c r="N61" t="inlineStr"/>
+      <c r="K63" t="n">
+        <v>3</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0.7351683908187316</v>
+      </c>
+      <c r="M63" t="n">
+        <v>6.484527183994263</v>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>15072</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" t="n">
+        <v>9</v>
+      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="n">
+        <v>5</v>
+      </c>
+      <c r="I64" t="n">
+        <v>150</v>
+      </c>
+      <c r="J64" t="n">
+        <v>55</v>
+      </c>
+      <c r="K64" t="n">
+        <v>7</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0.7385985299268407</v>
+      </c>
+      <c r="M64" t="n">
+        <v>6.505451032553728</v>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>HEK293</t>
+        </is>
+      </c>
+      <c r="O64" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DOTAP</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" t="n">
+        <v>12.515</v>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="n">
+        <v>6</v>
+      </c>
+      <c r="I65" t="n">
+        <v>150</v>
+      </c>
+      <c r="J65" t="n">
+        <v>35</v>
+      </c>
+      <c r="K65" t="n">
+        <v>3</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.7766742657825058</v>
+      </c>
+      <c r="M65" t="n">
+        <v>6.737713021273285</v>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>PC3</t>
+        </is>
+      </c>
+      <c r="O65" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31298</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>DOTAP</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="n">
+        <v>12.515</v>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="n">
+        <v>4</v>
+      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="n">
+        <v>6</v>
+      </c>
+      <c r="I66" t="n">
+        <v>150</v>
+      </c>
+      <c r="J66" t="n">
+        <v>45</v>
+      </c>
+      <c r="K66" t="n">
+        <v>3</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0.7766742657825058</v>
+      </c>
+      <c r="M66" t="n">
+        <v>6.737713021273285</v>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>N2a</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>28874</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>DOTAP</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" t="n">
+        <v>12.515</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>4</v>
+      </c>
+      <c r="G67" t="n">
+        <v>36</v>
+      </c>
+      <c r="H67" t="n">
+        <v>5</v>
+      </c>
+      <c r="I67" t="n">
+        <v>80</v>
+      </c>
+      <c r="J67" t="n">
+        <v>30</v>
+      </c>
+      <c r="K67" t="n">
+        <v>3</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0.8422277437855306</v>
+      </c>
+      <c r="M67" t="n">
+        <v>7.137589237091737</v>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>B16</t>
+        </is>
+      </c>
+      <c r="O67" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>26186</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="n">
+        <v>9</v>
+      </c>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="n">
+        <v>10</v>
+      </c>
+      <c r="I68" t="n">
+        <v>80</v>
+      </c>
+      <c r="J68" t="n">
+        <v>70</v>
+      </c>
+      <c r="K68" t="n">
+        <v>160</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0.8790140722709167</v>
+      </c>
+      <c r="M68" t="n">
+        <v>7.361985840852591</v>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>14608</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="n">
+        <v>9</v>
+      </c>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="n">
+        <v>5</v>
+      </c>
+      <c r="I69" t="n">
+        <v>80</v>
+      </c>
+      <c r="J69" t="n">
+        <v>75</v>
+      </c>
+      <c r="K69" t="n">
+        <v>3</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0.8799861653012702</v>
+      </c>
+      <c r="M69" t="n">
+        <v>7.367915608337746</v>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>28668</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="n">
+        <v>9</v>
+      </c>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="n">
+        <v>11</v>
+      </c>
+      <c r="I70" t="n">
+        <v>250</v>
+      </c>
+      <c r="J70" t="n">
+        <v>50</v>
+      </c>
+      <c r="K70" t="n">
+        <v>180</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0.9066252696552797</v>
+      </c>
+      <c r="M70" t="n">
+        <v>7.530414144897206</v>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>14765</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="n">
+        <v>9</v>
+      </c>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="n">
+        <v>5</v>
+      </c>
+      <c r="I71" t="n">
+        <v>200</v>
+      </c>
+      <c r="J71" t="n">
+        <v>30</v>
+      </c>
+      <c r="K71" t="n">
+        <v>5</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0.9135837784148289</v>
+      </c>
+      <c r="M71" t="n">
+        <v>7.572861048330456</v>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>26131</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="n">
+        <v>9</v>
+      </c>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="n">
+        <v>10</v>
+      </c>
+      <c r="I72" t="n">
+        <v>90</v>
+      </c>
+      <c r="J72" t="n">
+        <v>45</v>
+      </c>
+      <c r="K72" t="n">
+        <v>160</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0.9833729197174315</v>
+      </c>
+      <c r="M72" t="n">
+        <v>7.998574810276332</v>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>23740</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>DOPE</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" t="n">
+        <v>9.784000000000001</v>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="n">
+        <v>9</v>
+      </c>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="n">
+        <v>9</v>
+      </c>
+      <c r="I73" t="n">
+        <v>250</v>
+      </c>
+      <c r="J73" t="n">
+        <v>45</v>
+      </c>
+      <c r="K73" t="n">
+        <v>160</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0.9833729197174315</v>
+      </c>
+      <c r="M73" t="n">
+        <v>7.998574810276332</v>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>ARPE19</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>